<commit_message>
edited tests in FindDeclareTest
</commit_message>
<xml_diff>
--- a/docs/Aspekty.xlsx
+++ b/docs/Aspekty.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Аспекты тестирования" sheetId="2" r:id="rId1"/>
@@ -2098,8 +2098,8 @@
   <sheetPr/>
   <dimension ref="A1:XFD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
@@ -31146,8 +31146,8 @@
   <sheetPr/>
   <dimension ref="A1:IV51"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
@@ -32741,7 +32741,7 @@
         <v>31</v>
       </c>
       <c r="C7" s="30">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="38" t="s">
         <v>78</v>

</xml_diff>